<commit_message>
Completed Kubernetes for beginners course
</commit_message>
<xml_diff>
--- a/202108_Docker/202205_Kubernetes.xlsx
+++ b/202108_Docker/202205_Kubernetes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\202108_Docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDCDDD9-BEB7-4180-BBB9-E532CF6F1576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A21AD16-D82A-40D5-B03C-ED22B2FF0422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="S4-6.Concepts" sheetId="3" r:id="rId3"/>
     <sheet name="S5.YAML" sheetId="5" r:id="rId4"/>
     <sheet name="S7.Networks" sheetId="6" r:id="rId5"/>
-    <sheet name="S8-9.Service" sheetId="7" r:id="rId6"/>
-    <sheet name="S10.Cloud" sheetId="4" r:id="rId7"/>
+    <sheet name="S8.Service" sheetId="7" r:id="rId6"/>
+    <sheet name="S9.Microservice" sheetId="8" r:id="rId7"/>
+    <sheet name="S10.Cloud" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="501">
   <si>
     <t>Course 1</t>
   </si>
@@ -334,9 +335,6 @@
     <t>Cloud</t>
   </si>
   <si>
-    <t>GCP / AWS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Practice </t>
   </si>
   <si>
@@ -724,6 +722,9 @@
     <t>// Dictionary</t>
   </si>
   <si>
+    <t xml:space="preserve">     app: myapp</t>
+  </si>
+  <si>
     <t xml:space="preserve">  name: myapp-pod</t>
   </si>
   <si>
@@ -770,6 +771,9 @@
   </si>
   <si>
     <t xml:space="preserve">  - name: postgres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    image: postgres</t>
   </si>
   <si>
     <t xml:space="preserve">     image: postgres</t>
@@ -1232,9 +1236,6 @@
     <t>S7</t>
   </si>
   <si>
-    <t>S8-9</t>
-  </si>
-  <si>
     <t>S10</t>
   </si>
   <si>
@@ -1275,6 +1276,860 @@
   </si>
   <si>
     <t>$ kubectl get nodes -o wide</t>
+  </si>
+  <si>
+    <t>Services enable communication within and outside application.</t>
+  </si>
+  <si>
+    <t>Services enable loose coupling between micro-services.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For  example, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>service listens to a port on a node</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>and forward request on that port =&gt; NodePort service</t>
+  </si>
+  <si>
+    <t>NodePort</t>
+  </si>
+  <si>
+    <t>Make an internal POD accessible on a Node Port</t>
+  </si>
+  <si>
+    <t>ClusterIP</t>
+  </si>
+  <si>
+    <t>create a virtual IP inside cluster</t>
+  </si>
+  <si>
+    <t>enable communication between different services</t>
+  </si>
+  <si>
+    <t>LoadBalancer</t>
+  </si>
+  <si>
+    <t>provision a load balancer for service in support cloud providers</t>
+  </si>
+  <si>
+    <t>Services: NodePort, ClusterIP, LoadBalancer;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TargetPort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Port on POD where actual server running</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Port</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Port on Service itself</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NodePort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Port on Node which we use to access the Web externally</t>
+    </r>
+  </si>
+  <si>
+    <t>service-definition.yaml</t>
+  </si>
+  <si>
+    <r>
+      <t>kind:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Service</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  name: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>myapp-service</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  type: NodePort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ports:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     - targetPort: 80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       nodePort: 30008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       port: 80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     type: front-end</t>
+  </si>
+  <si>
+    <t>$ kubectl create -f service-definition.yaml</t>
+  </si>
+  <si>
+    <t>$ kubectl get services</t>
+  </si>
+  <si>
+    <t>// map the PODs to Service</t>
+  </si>
+  <si>
+    <t>How the ports are distributed across multiple nodes</t>
+  </si>
+  <si>
+    <t>Kubernetes creates a service that spans across all the nodes in the cluster.</t>
+  </si>
+  <si>
+    <t>and maps the TargetPort (ex 80) to the SAME NodePort (ex 30008) on all nodes in the cluster.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">=&gt; We can access our app </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>using the IP of any node with the same port number.</t>
+    </r>
+  </si>
+  <si>
+    <t>$ minikube service myapp-service --url</t>
+  </si>
+  <si>
+    <t>The requests are forwareded to one of the PODs randomly.</t>
+  </si>
+  <si>
+    <t>The name should be used by other PODs to access the service.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  name: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>myapp-service-clusterip</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  type: ClusterIP</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Each service gets </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>an IP and name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> inside the cluster.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ClusterIP service groups PODs together and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>provide a single interface</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>This only work with supported cloud platforms (GCP, AWS, Azure)</t>
+  </si>
+  <si>
+    <t>External load balancer configuration.</t>
+  </si>
+  <si>
+    <t>On local environment, it works like NodePort</t>
+  </si>
+  <si>
+    <t>$ kubectl describe service myapp-service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        port: 30008</t>
+  </si>
+  <si>
+    <t>// POD port</t>
+  </si>
+  <si>
+    <t>// service port</t>
+  </si>
+  <si>
+    <t>// node port</t>
+  </si>
+  <si>
+    <t>$ kubectl expose deployment simple-webapp-deployment --name=webapp-service /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   --target-port=8080 --type=NodePort --port=8080 --dry-run=client -o yaml &gt; svc.yaml</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>Self Hosted / Turnkey Solution</t>
+  </si>
+  <si>
+    <t>Hosted Solutions / Managed Solutions</t>
+  </si>
+  <si>
+    <t>Kubernetes-as-a-service</t>
+  </si>
+  <si>
+    <t>Provider provisions VMs</t>
+  </si>
+  <si>
+    <t>Provider installs Kubernetes</t>
+  </si>
+  <si>
+    <t>Provider maintains VMs</t>
+  </si>
+  <si>
+    <t>We provision VMs</t>
+  </si>
+  <si>
+    <t>We configure VMs</t>
+  </si>
+  <si>
+    <t>We use scripts to deploy cluster</t>
+  </si>
+  <si>
+    <t>We maintain VMs ourselves</t>
+  </si>
+  <si>
+    <t>Note: we don’t have access to Master Node/VMs</t>
+  </si>
+  <si>
+    <t>Hosted Solutions</t>
+  </si>
+  <si>
+    <t>Google Kubernetes Engine (GKE)</t>
+  </si>
+  <si>
+    <t>Azure Kubernetes Service (AKS)</t>
+  </si>
+  <si>
+    <t>Amazon Elastic Kubernetes Service (EKS)</t>
+  </si>
+  <si>
+    <t>GKE</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/free/</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/kubernetes-engine/docs/</t>
+  </si>
+  <si>
+    <t>EKS</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>https://github.com/dockersamples/example-voting-app</t>
+  </si>
+  <si>
+    <t>https://github.com/mmumshad/example-voting-app-kubernetes-v2</t>
+  </si>
+  <si>
+    <t>$ kubectl exec -it POD_NAME -- /bin/bash</t>
+  </si>
+  <si>
+    <t>AKS</t>
+  </si>
+  <si>
+    <t>GCP / AWS / Azure</t>
+  </si>
+  <si>
+    <t>https://kubernetes.io/docs/setup/independent/install-kubeadm/</t>
+  </si>
+  <si>
+    <t>Kubeadm</t>
+  </si>
+  <si>
+    <t>helps us setup a multi-node cluster following Kubernetes best practices.</t>
+  </si>
+  <si>
+    <t>Step 1: Provision multiple systems or VMs for configuring a cluster.</t>
+  </si>
+  <si>
+    <t>Step 2: Designate one node as Master, and others as Worker nodes.</t>
+  </si>
+  <si>
+    <t>Step 3: Install docker runtime on the hosts.</t>
+  </si>
+  <si>
+    <t>Step 4: Install Kubeadm tool on all the nodes.</t>
+  </si>
+  <si>
+    <t>Step 5: Initialize the Master server.</t>
+  </si>
+  <si>
+    <t>must ensure that network prerequisites are met, POD network.</t>
+  </si>
+  <si>
+    <t>Step 6: Join the worker node to Master node.</t>
+  </si>
+  <si>
+    <t>S1-3.Overview'!A150</t>
+  </si>
+  <si>
+    <t>Sample application</t>
+  </si>
+  <si>
+    <t>voting app</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>worker</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>result-app</t>
+  </si>
+  <si>
+    <t>front-end app which lets us vote between two options</t>
+  </si>
+  <si>
+    <t>queue which collects new votes</t>
+  </si>
+  <si>
+    <t>worker which consumes votes and store them in db</t>
+  </si>
+  <si>
+    <t>database backed by a Docker volume</t>
+  </si>
+  <si>
+    <t>webapp which shows the results of the voting in real time</t>
+  </si>
+  <si>
+    <t>Remember docker…</t>
+  </si>
+  <si>
+    <t>docker run -d --name=redis redis</t>
+  </si>
+  <si>
+    <t>docker run -d --name=db postgres:9.4</t>
+  </si>
+  <si>
+    <t>docker run -d --name=vote -p 5000:80 --link redis:redis voting-app</t>
+  </si>
+  <si>
+    <t>docker run -d --name=result -p 5001:80 --link db:db result-app</t>
+  </si>
+  <si>
+    <t>docker run -d --name=worker --link db:db --link redis:redis worker</t>
+  </si>
+  <si>
+    <t>Goals:</t>
+  </si>
+  <si>
+    <t>1 - Deploy containers</t>
+  </si>
+  <si>
+    <t>2 - Enable connectivity</t>
+  </si>
+  <si>
+    <t>3 - External Access</t>
+  </si>
+  <si>
+    <t>Steps:</t>
+  </si>
+  <si>
+    <t>1 - Deploy PODs</t>
+  </si>
+  <si>
+    <t>2 - Create Services (ClusterIP)</t>
+  </si>
+  <si>
+    <t>1. redis; 2. db;</t>
+  </si>
+  <si>
+    <t>3 - Create Services (NodePort)</t>
+  </si>
+  <si>
+    <t>1. voting-app; 2. result-app</t>
+  </si>
+  <si>
+    <t>Deploy microservices app</t>
+  </si>
+  <si>
+    <t>Microservices app on Kubernetes</t>
+  </si>
+  <si>
+    <t>voting-app-pod.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: voting-app-pod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    name: voting-app-pod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - name: voting-app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    image: kodekloud/examplevotingapp_vote:v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ports:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      - containerPort: 80</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>apiVersion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: v1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kind</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Pod</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>metadata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>result-app-pod.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: result-app-pod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    name: result-app-pod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - name: result-app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    image: kodekloud/examplevotingapp_result:v1</t>
+  </si>
+  <si>
+    <t>redis-pod.yaml</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    app: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>demo-voting-app</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: redis-pod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - name: redis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    image: redis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      - containerPort: 6379</t>
+  </si>
+  <si>
+    <t>postgres-pod.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: postgres-pod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    name: postgres-pod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    name: redis-pod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      - containerPort: 5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    env:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      - name: POSTGRES_USER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        value: "postgres"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      - name: POSTGRES_PASSWORD</t>
+  </si>
+  <si>
+    <t>worker-pod.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: worker-pod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - name: worker-app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    image: kodekloud/examplevotingapp_worker:v1</t>
+  </si>
+  <si>
+    <t>redis-service.yaml</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kind</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Service</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: redis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    name: redis-service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - port: 6379</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      targetPort: 6379</t>
+  </si>
+  <si>
+    <t>postgres-service.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: db</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    name: postgres-service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      targetPort: 5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - port: 5432</t>
+  </si>
+  <si>
+    <t>voting-app-service.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: voting-service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    name: voting-service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - port: 80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      targetPort: 80</t>
+  </si>
+  <si>
+    <t>result-app-service.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  name: result-service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    name: result-service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  type: NotePort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      nodePort: 30004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      nodePort: 30005</t>
+  </si>
+  <si>
+    <t>$ kubectl get pods,svc</t>
+  </si>
+  <si>
+    <t>$ minikube service voting-service --url</t>
+  </si>
+  <si>
+    <t>$ minikube service result-service --url</t>
+  </si>
+  <si>
+    <t>=&gt; http://192.168.99.101:30004</t>
+  </si>
+  <si>
+    <t>=&gt; http://192.168.99.101:30005</t>
+  </si>
+  <si>
+    <t>Deploy microservices app with Deployments</t>
+  </si>
+  <si>
+    <t>Microservices;</t>
+  </si>
+  <si>
+    <t>Deploy microservices with PODs and Services;</t>
+  </si>
+  <si>
+    <t>Deploy microservices with Deployments;</t>
+  </si>
+  <si>
+    <t>Deployment helps us perform rolling updates and rollbacks and maintain a record of revisions.</t>
   </si>
 </sst>
 </file>
@@ -1433,7 +2288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1464,6 +2319,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1806,13 +2662,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>504305</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>161665</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1850,13 +2706,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>323617</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>142715</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1894,13 +2750,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>275992</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>133190</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1938,13 +2794,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>140</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>589714</xdr:colOff>
-      <xdr:row>147</xdr:row>
+      <xdr:row>149</xdr:row>
       <xdr:rowOff>171214</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1982,13 +2838,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>171</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>523048</xdr:colOff>
-      <xdr:row>179</xdr:row>
+      <xdr:row>181</xdr:row>
       <xdr:rowOff>133095</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2151,6 +3007,280 @@
         <a:xfrm>
           <a:off x="6096000" y="771525"/>
           <a:ext cx="3405187" cy="2105025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2511</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1C8BCE5-1C89-4A46-A6E7-2D9449D2A4D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486401" y="962025"/>
+          <a:ext cx="3486149" cy="1726536"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>456686</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68B51D15-3A70-4C32-9D2E-1D9C157B729C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="3067050"/>
+          <a:ext cx="4114286" cy="2009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>13621</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D02FCBE-4394-4B51-B683-9A77F74CA73A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486401" y="5353051"/>
+          <a:ext cx="3676650" cy="1918620"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561524</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>161619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D0E27C5-5BD3-4DC6-A69F-2752B22BEBB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="11830050"/>
+          <a:ext cx="3609524" cy="2447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>132631</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8342BC93-231F-4609-88BF-583C6FB3A7A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="16021051"/>
+          <a:ext cx="3790231" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>78460</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D2A255F-D898-47E9-871C-33292150CBFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="962026"/>
+          <a:ext cx="2516860" cy="2085974"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2428,7 +3558,7 @@
   <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2441,7 +3571,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -2449,7 +3579,7 @@
         <v>2</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -2503,7 +3633,7 @@
         <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -2525,7 +3655,7 @@
         <v>22</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -2536,7 +3666,7 @@
         <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -2546,6 +3676,9 @@
       <c r="C14" t="s">
         <v>24</v>
       </c>
+      <c r="I14" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -2566,12 +3699,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -2584,8 +3720,10 @@
     <hyperlink ref="M3" r:id="rId2" xr:uid="{667563B1-9C4D-4FE2-9A96-1041C3511CF5}"/>
     <hyperlink ref="I11" location="'S4-6.Concepts'!A50" display="S4-6" xr:uid="{6B95942C-010A-417C-AE50-9B476E6C5A01}"/>
     <hyperlink ref="I12" location="S7.Networks!A1" display="S7" xr:uid="{F72927CD-C311-4396-BB49-F9AA4975356E}"/>
-    <hyperlink ref="I13" location="'S8-9.Service'!A1" display="S8-9" xr:uid="{E50AE415-15D6-440B-85A4-64AAFBBC8917}"/>
+    <hyperlink ref="I13" location="S8.Service!A1" display="S8" xr:uid="{E50AE415-15D6-440B-85A4-64AAFBBC8917}"/>
     <hyperlink ref="I15" location="S10.Cloud!A1" display="S10" xr:uid="{0F911F41-8B27-442A-9836-682014819204}"/>
+    <hyperlink ref="I14" location="S9.Microservice!A1" display="S9" xr:uid="{7350715F-597E-41F4-85F3-55691363D7BE}"/>
+    <hyperlink ref="I17" location="'S1-3.Overview'!A150" display="'S1-3.Overview'!A150" xr:uid="{1DBD05E7-A39E-4210-A410-C927F7472E59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -2594,10 +3732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB6F0CA-2F5D-4605-8C36-B2178CBE30E9}">
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,17 +3745,17 @@
         <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2975,19 +4113,19 @@
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D115" t="s">
+      <c r="D115" s="8" t="s">
         <v>89</v>
       </c>
       <c r="F115" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D116" t="s">
+      <c r="D116" s="8" t="s">
         <v>90</v>
       </c>
       <c r="F116" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
@@ -2997,17 +4135,17 @@
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>92</v>
+        <v>393</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
@@ -3017,100 +4155,159 @@
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D136" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D137" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D139" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D140" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D141" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D142" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B146" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C147" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B149" s="5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C150" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E156" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="Intro!A1" display="Intro!A1" xr:uid="{2BDB687A-25E9-4017-99DD-104FC59EBA07}"/>
     <hyperlink ref="D136" r:id="rId1" xr:uid="{831C8923-FF1E-46D7-BD45-26F693C8C556}"/>
+    <hyperlink ref="C147" r:id="rId2" xr:uid="{D5A03B8E-E713-473C-BE70-D06927F7BC02}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE62828F-30AF-43A0-8C08-890DC7487EDB}">
-  <dimension ref="A1:O188"/>
+  <dimension ref="A1:O190"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="G182" sqref="G182"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3120,17 +4317,17 @@
         <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3143,67 +4340,67 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -3213,42 +4410,42 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="2:15" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3261,64 +4458,64 @@
     </row>
     <row r="46" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C47" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M47" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N47" s="19"/>
       <c r="O47" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D48" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F48" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M48" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N48" s="17"/>
       <c r="O48" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F49" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M49" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N49" s="17"/>
       <c r="O49" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D50" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M50" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N50" s="17"/>
       <c r="O50" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="4:15" x14ac:dyDescent="0.25">
@@ -3326,11 +4523,11 @@
         <v>210</v>
       </c>
       <c r="M51" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N51" s="17"/>
       <c r="O51" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="4:15" x14ac:dyDescent="0.25">
@@ -3338,7 +4535,7 @@
         <v>211</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="4:15" x14ac:dyDescent="0.25">
@@ -3358,10 +4555,10 @@
     </row>
     <row r="56" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D56" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="4:15" x14ac:dyDescent="0.25">
@@ -3369,7 +4566,7 @@
         <v>212</v>
       </c>
       <c r="H57" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="4:15" x14ac:dyDescent="0.25">
@@ -3377,7 +4574,7 @@
         <v>213</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="4:15" x14ac:dyDescent="0.25">
@@ -3390,20 +4587,20 @@
         <v>225</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="4:15" x14ac:dyDescent="0.25">
@@ -3413,362 +4610,357 @@
     </row>
     <row r="64" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G73" s="14" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="8" t="s">
+      <c r="C75" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C77" s="8" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E79" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="82" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B82" s="5" t="s">
+    <row r="84" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D87" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C93" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="I93" s="8" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C94" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="I94" s="11" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D95" s="8" t="s">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C95" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="I95" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C96" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="I96" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D97" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="J97" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="J95" s="8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D96" s="8" t="s">
+    </row>
+    <row r="98" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D98" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="J98" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="J96" s="8" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="97" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D97" s="8" t="s">
+    </row>
+    <row r="99" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D99" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="J99" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="100" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>269</v>
+      </c>
+      <c r="J100" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="101" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>211</v>
+      </c>
+      <c r="J101" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="102" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>223</v>
+      </c>
+      <c r="J102" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="103" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>248</v>
+      </c>
+      <c r="J103" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="104" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D104" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="J97" s="8" t="s">
+      <c r="J104" s="8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
-        <v>268</v>
-      </c>
-      <c r="J98" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="99" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D99" t="s">
-        <v>211</v>
-      </c>
-      <c r="J99" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="100" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D100" t="s">
-        <v>223</v>
-      </c>
-      <c r="J100" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="101" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D101" t="s">
-        <v>247</v>
-      </c>
-      <c r="J101" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="102" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D102" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="J102" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="103" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D103" t="s">
-        <v>274</v>
-      </c>
-      <c r="J103" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="104" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
-        <v>249</v>
-      </c>
-      <c r="J104" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="105" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D105" t="s">
-        <v>249</v>
+        <v>275</v>
       </c>
       <c r="J105" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="106" spans="4:13" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="106" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J106" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="107" spans="4:13" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="107" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J107" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="108" spans="4:13" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="108" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J108" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="109" spans="4:13" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="109" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J109" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="110" spans="4:13" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="110" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J110" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="111" spans="4:13" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="111" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="J111" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="112" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="J112" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="112" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>250</v>
+      </c>
+      <c r="J112" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="113" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
         <v>276</v>
       </c>
-      <c r="M112" s="13" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="113" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="J113" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="M113" s="13" t="s">
-        <v>257</v>
+      <c r="J113" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="114" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J114" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="M114" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="115" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J115" s="6" t="s">
         <v>255</v>
       </c>
+      <c r="M115" s="13" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="116" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C116" t="s">
-        <v>248</v>
-      </c>
-      <c r="J116" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="117" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C117" t="s">
-        <v>250</v>
-      </c>
-      <c r="J117" t="s">
+      <c r="J116" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="118" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>249</v>
+      </c>
+      <c r="J118" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="118" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="J118" t="s">
-        <v>277</v>
-      </c>
-    </row>
     <row r="119" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>251</v>
+      </c>
       <c r="J119" t="s">
-        <v>278</v>
-      </c>
-      <c r="O119" s="14" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
     </row>
     <row r="120" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J120" t="s">
-        <v>271</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="121" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J121" t="s">
+        <v>279</v>
+      </c>
+      <c r="O121" s="14" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="122" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C122" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="123" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D123" t="s">
-        <v>262</v>
+      <c r="J122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="124" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C124" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="125" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C125" s="2" t="s">
+      <c r="D125" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="126" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D126" t="s">
+    <row r="127" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C127" s="2" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="127" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="E127" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="128" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E129" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E130" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B133" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C134" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C135" t="s">
-        <v>283</v>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E132" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B135" s="5" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
@@ -3778,47 +4970,47 @@
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="150" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C150" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="151" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C151" s="11" t="s">
-        <v>286</v>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C139" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="152" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D152" s="8" t="s">
-        <v>272</v>
+      <c r="C152" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="153" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D153" s="8" t="s">
-        <v>285</v>
+      <c r="C153" s="11" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="154" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D154" s="8" t="s">
-        <v>193</v>
+        <v>273</v>
       </c>
     </row>
     <row r="155" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D155" t="s">
-        <v>290</v>
+      <c r="D155" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="156" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="8" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="157" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C157" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C158" t="s">
-        <v>302</v>
+      <c r="D157" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="159" spans="3:4" x14ac:dyDescent="0.25">
@@ -3828,26 +5020,31 @@
     </row>
     <row r="160" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="164" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B164" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C166" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C162" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C163" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B166" s="5" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C167" t="s">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C168" t="s">
         <v>293</v>
       </c>
     </row>
@@ -3856,37 +5053,42 @@
         <v>294</v>
       </c>
     </row>
-    <row r="182" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C182" s="8" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="183" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C183" t="s">
-        <v>296</v>
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C171" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="184" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C184" t="s">
-        <v>297</v>
+      <c r="C184" s="8" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="185" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C185" t="s">
-        <v>289</v>
-      </c>
-      <c r="I185" s="14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="186" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C186" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="187" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C187" s="8" t="s">
+      <c r="C187" t="s">
+        <v>290</v>
+      </c>
+      <c r="I187" s="14" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="188" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C188" t="s">
+    <row r="189" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C189" s="8" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="190" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C190" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -3925,10 +5127,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3941,221 +5143,221 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F14" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D17" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -4171,8 +5373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73469F42-6832-4A87-A6AC-B1EDF113AC07}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4246,27 +5448,1179 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A2D505-2412-4CAE-AA38-79AD3C1C40A3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="8" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D36" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D37" s="8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D38" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D42" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D43" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D44" s="6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D45" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D46" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D47" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D48" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D81" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="G81" s="14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D82" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D83" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="G83" s="14" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D84" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D85" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C90" s="12" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>359</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Intro!A1" display="Intro!A1" xr:uid="{A4FB059D-59A8-4118-BF6B-FDA60E12987A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887204C1-90B6-4BD8-9B5E-626C776F2178}">
-  <dimension ref="B4:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1863C95-18D0-4680-8DF0-7B9D3F880515}">
+  <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>406</v>
+      </c>
+      <c r="E7" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>407</v>
+      </c>
+      <c r="E8" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>408</v>
+      </c>
+      <c r="E9" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>409</v>
+      </c>
+      <c r="E10" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>410</v>
+      </c>
+      <c r="E11" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>388</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>422</v>
+      </c>
+      <c r="D25" t="s">
+        <v>423</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="H25" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>424</v>
+      </c>
+      <c r="H26" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>425</v>
+      </c>
+      <c r="I27" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C33" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>441</v>
+      </c>
+      <c r="K34" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>442</v>
+      </c>
+      <c r="K35" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>443</v>
+      </c>
+      <c r="K36" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>435</v>
+      </c>
+      <c r="K37" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>211</v>
+      </c>
+      <c r="K38" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>436</v>
+      </c>
+      <c r="K39" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>451</v>
+      </c>
+      <c r="K40" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>444</v>
+      </c>
+      <c r="K41" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>212</v>
+      </c>
+      <c r="K42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>437</v>
+      </c>
+      <c r="K43" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>438</v>
+      </c>
+      <c r="K44" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>439</v>
+      </c>
+      <c r="K45" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>440</v>
+      </c>
+      <c r="K46" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C48" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>441</v>
+      </c>
+      <c r="K49" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>442</v>
+      </c>
+      <c r="K50" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>443</v>
+      </c>
+      <c r="K51" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>452</v>
+      </c>
+      <c r="K52" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>211</v>
+      </c>
+      <c r="K53" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>459</v>
+      </c>
+      <c r="K54" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>451</v>
+      </c>
+      <c r="K55" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>444</v>
+      </c>
+      <c r="K56" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>212</v>
+      </c>
+      <c r="K57" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>453</v>
+      </c>
+      <c r="K58" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>454</v>
+      </c>
+      <c r="K59" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>439</v>
+      </c>
+      <c r="K60" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>455</v>
+      </c>
+      <c r="K61" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="62" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K62" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="63" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K63" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K64" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K65" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K66" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C68" s="11" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="69" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="70" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="71" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="72" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="73" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="74" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="75" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="76" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="77" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="78" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="79" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="80" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C80" s="22"/>
+    </row>
+    <row r="81" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C81" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="J81" s="11" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="82" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>441</v>
+      </c>
+      <c r="K82" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="83" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>470</v>
+      </c>
+      <c r="K83" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="84" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>443</v>
+      </c>
+      <c r="K84" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="85" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>471</v>
+      </c>
+      <c r="K85" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="86" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>211</v>
+      </c>
+      <c r="K86" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>472</v>
+      </c>
+      <c r="K87" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="88" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>451</v>
+      </c>
+      <c r="K88" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="89" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>444</v>
+      </c>
+      <c r="K89" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="90" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>338</v>
+      </c>
+      <c r="K90" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="91" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>473</v>
+      </c>
+      <c r="K91" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="92" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>474</v>
+      </c>
+      <c r="K92" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="93" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>277</v>
+      </c>
+      <c r="K93" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="94" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>459</v>
+      </c>
+      <c r="K94" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="95" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>451</v>
+      </c>
+      <c r="K95" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="97" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C97" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="J97" s="11" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="98" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>441</v>
+      </c>
+      <c r="K98" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="99" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>470</v>
+      </c>
+      <c r="K99" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="100" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>443</v>
+      </c>
+      <c r="K100" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="101" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>481</v>
+      </c>
+      <c r="K101" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="102" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>211</v>
+      </c>
+      <c r="K102" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="103" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>482</v>
+      </c>
+      <c r="K103" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="104" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>451</v>
+      </c>
+      <c r="K104" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="105" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>444</v>
+      </c>
+      <c r="K105" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="106" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>488</v>
+      </c>
+      <c r="K106" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="107" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>338</v>
+      </c>
+      <c r="K107" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="108" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>483</v>
+      </c>
+      <c r="K108" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="109" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>484</v>
+      </c>
+      <c r="K109" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="110" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>489</v>
+      </c>
+      <c r="K110" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="111" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>277</v>
+      </c>
+      <c r="K111" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="112" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>436</v>
+      </c>
+      <c r="K112" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>451</v>
+      </c>
+      <c r="K113" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>492</v>
+      </c>
+      <c r="H116" s="14" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>493</v>
+      </c>
+      <c r="H117" s="14" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B120" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Intro!A1" display="Intro!A1" xr:uid="{93417D2B-5EAE-42A0-BD8E-750385716633}"/>
+    <hyperlink ref="D13" r:id="rId1" xr:uid="{21434F2F-F934-4768-9929-6DE191D87F31}"/>
+    <hyperlink ref="D14" r:id="rId2" xr:uid="{E8E4B71E-A090-45DB-9971-D3205142C89F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887204C1-90B6-4BD8-9B5E-626C776F2178}">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -4274,7 +6628,110 @@
         <v>25</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>375</v>
+      </c>
+      <c r="H8" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>376</v>
+      </c>
+      <c r="H9" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>378</v>
+      </c>
+      <c r="H11" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Intro!A1" display="Intro!A1" xr:uid="{50CA08AD-40E1-463E-8318-242BB5CF95A5}"/>
+    <hyperlink ref="C21" r:id="rId1" xr:uid="{110D212A-A3CB-4E47-BA5F-1031E0B49542}"/>
+    <hyperlink ref="C22" r:id="rId2" xr:uid="{17998592-23AE-4D86-846B-1C9A56D52798}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
k8s: demo server return ip address of kubernetes pod
</commit_message>
<xml_diff>
--- a/202108_Docker/202205_Kubernetes.xlsx
+++ b/202108_Docker/202205_Kubernetes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\202108_Docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A21AD16-D82A-40D5-B03C-ED22B2FF0422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402B0CA0-0E92-4BF8-9C5C-2D13CEA120A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <sheet name="S8.Service" sheetId="7" r:id="rId6"/>
     <sheet name="S9.Microservice" sheetId="8" r:id="rId7"/>
     <sheet name="S10.Cloud" sheetId="4" r:id="rId8"/>
+    <sheet name="Practice" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="566">
   <si>
     <t>Course 1</t>
   </si>
@@ -344,9 +345,6 @@
     <t>providing us a pre-configured single node kubernetes cluster</t>
   </si>
   <si>
-    <t>Minikube bundles all of Kubernetes different components into a single image (ISO),</t>
-  </si>
-  <si>
     <t>Requirement:</t>
   </si>
   <si>
@@ -1282,32 +1280,6 @@
   </si>
   <si>
     <t>Services enable loose coupling between micro-services.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For  example, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>service listens to a port on a node</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
   </si>
   <si>
     <t>and forward request on that port =&gt; NodePort service</t>
@@ -1409,9 +1381,6 @@
     </r>
   </si>
   <si>
-    <t>service-definition.yaml</t>
-  </si>
-  <si>
     <r>
       <t>kind:</t>
     </r>
@@ -1468,9 +1437,6 @@
   </si>
   <si>
     <t xml:space="preserve">     type: front-end</t>
-  </si>
-  <si>
-    <t>$ kubectl create -f service-definition.yaml</t>
   </si>
   <si>
     <t>$ kubectl get services</t>
@@ -1722,9 +1688,6 @@
   </si>
   <si>
     <t>Step 6: Join the worker node to Master node.</t>
-  </si>
-  <si>
-    <t>S1-3.Overview'!A150</t>
   </si>
   <si>
     <t>Sample application</t>
@@ -2131,12 +2094,519 @@
   <si>
     <t>Deployment helps us perform rolling updates and rollbacks and maintain a record of revisions.</t>
   </si>
+  <si>
+    <t>Step 1: Build test server docker image</t>
+  </si>
+  <si>
+    <t>$ docker build -t tung-server .</t>
+  </si>
+  <si>
+    <t>$ docker run -d --name tung-server1 -p 8081:8080 tung-server</t>
+  </si>
+  <si>
+    <t>Verify server</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Minikube bundles all of Kubernetes different components into </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a single image (ISO)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>S1-3!A150</t>
+  </si>
+  <si>
+    <t>Practice</t>
+  </si>
+  <si>
+    <t>DEMO 1 - Use kubectl to deploy a test server (Pod, Deployment, ReplicaSet, Service)</t>
+  </si>
+  <si>
+    <t>TROUBLESHOOT 1: Error: ImagePullBackOff</t>
+  </si>
+  <si>
+    <t>failed to pull and unpack image "docker.io/library/tung-server:latest"</t>
+  </si>
+  <si>
+    <t>[NOT WORK] https://stackoverflow.com/questions/57167104/how-to-use-local-docker-image-in-kubernetes-via-kubectl</t>
+  </si>
+  <si>
+    <t>=&gt; Deploy image to ACR</t>
+  </si>
+  <si>
+    <t>$ az login</t>
+  </si>
+  <si>
+    <t>Access keys &gt;&gt; Enable Admin user</t>
+  </si>
+  <si>
+    <t>$ az acr login --name tungkuberegistry --username tungkuberegistry --password xxxxxx</t>
+  </si>
+  <si>
+    <t>$ docker push tungkuberegistry.azurecr.io/tung-server</t>
+  </si>
+  <si>
+    <t>Step 2: Deploy image to Azure container registry</t>
+  </si>
+  <si>
+    <t>Create tung-server-pod.yaml file</t>
+  </si>
+  <si>
+    <t>$ kubectl create -f tung-server-pod.yaml</t>
+  </si>
+  <si>
+    <t>Step 3: Create AKS cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    --node-count 2 --generate-ssh-keys --attach-acr tungkuberegistry</t>
+  </si>
+  <si>
+    <t>$ az aks get-credentials --resource-group CAP --name cap-azurecni-public --admin</t>
+  </si>
+  <si>
+    <t>$ kubectl apply -f tung-server-pod.yaml</t>
+  </si>
+  <si>
+    <t>$ kubectl describe pod tung-app-pod</t>
+  </si>
+  <si>
+    <t>=&gt; tung-app-pod   1/1     Running   0          29s</t>
+  </si>
+  <si>
+    <t>Verify application running properly</t>
+  </si>
+  <si>
+    <t>Step 4: Run POD yaml</t>
+  </si>
+  <si>
+    <t>Step 5: Run Deployment yaml</t>
+  </si>
+  <si>
+    <t>Try to delete a pod:</t>
+  </si>
+  <si>
+    <t>$ kubectl delete pod tung-app-deployment-5665977898-5m6l2</t>
+  </si>
+  <si>
+    <t>=&gt; new pod automatically created</t>
+  </si>
+  <si>
+    <t>Try to change replica 3 -&gt; 2:</t>
+  </si>
+  <si>
+    <t>$ kubectl apply -f tung-server-deployment.yaml</t>
+  </si>
+  <si>
+    <t>$ kubectl get pods,deployments</t>
+  </si>
+  <si>
+    <t>=&gt; One pod is auto deleted</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ az group create --name </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tung-kube-rg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --location australiaeast</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ az acr create --resource-group tung-kube-rg --name </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tungkuberegistry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --sku Basic</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ docker tag tung-server </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tungkuberegistry.azurecr.io/tung-server</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ az aks create --resource-group tung-kube-rg --name </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tungAKSCluster</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> \</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> my_pod_ip_address[10.244.1.5:8080]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For  example, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>service listens to port 30008 on a node</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kubectl debug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> node/aks-nodepool1-19874846-vmss000001 -it --image=busybox</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kubectl exec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -it tung-app-deployment-5665977898-g6tdh -- sh</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kubectl create</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -f tung-server-deployment.yaml</t>
+    </r>
+  </si>
+  <si>
+    <t>Step 6: Run NodePort Service yaml</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kubectl create</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -f tung-server-nodePort.yaml</t>
+    </r>
+  </si>
+  <si>
+    <t>$ kubectl get pods,deployments,svc</t>
+  </si>
+  <si>
+    <t>Verify node port service running properly</t>
+  </si>
+  <si>
+    <t>$ wget localhost:30008</t>
+  </si>
+  <si>
+    <t>  name: azure-vote-front</t>
+  </si>
+  <si>
+    <t>  ports:</t>
+  </si>
+  <si>
+    <t>  - port: 80</t>
+  </si>
+  <si>
+    <t>  selector:</t>
+  </si>
+  <si>
+    <t>    app: azure-vote-front</t>
+  </si>
+  <si>
+    <t>service-loadbalancer-definition.yaml</t>
+  </si>
+  <si>
+    <t>service-nodeport-definition.yaml</t>
+  </si>
+  <si>
+    <t>$ kubectl create -f service-nodeport-definition.yaml</t>
+  </si>
+  <si>
+    <t>service-clusterIP-definition.yaml</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>apiVersion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> v1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kind:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Service</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  type: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LoadBalancer</t>
+    </r>
+  </si>
+  <si>
+    <t>Demo server functionality</t>
+  </si>
+  <si>
+    <t>Step 7: Run LoadBalancer Service yaml</t>
+  </si>
+  <si>
+    <t>$ kubectl.exe create -f tung-server-loadBalancer.yaml</t>
+  </si>
+  <si>
+    <t>$ kubectl get pods,deployment,svc</t>
+  </si>
+  <si>
+    <t>Access http://20.53.190.36:8080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REQ-1: Listen on port 8080 </t>
+  </si>
+  <si>
+    <t>REQ-2: Return the network interface of container</t>
+  </si>
+  <si>
+    <t>https://github.com/kodekloudhub/example-voting-app-kubernetes</t>
+  </si>
+  <si>
+    <t>// default service if type is not defined</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2209,6 +2679,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2288,7 +2773,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2305,21 +2790,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2662,13 +3148,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>504305</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>161665</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2706,13 +3192,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>323617</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>142715</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2750,13 +3236,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>275992</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>133190</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2794,13 +3280,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>589714</xdr:colOff>
-      <xdr:row>149</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>171214</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2838,13 +3324,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>523048</xdr:colOff>
-      <xdr:row>181</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>133095</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3023,15 +3509,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>2</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>2511</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>208132</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3054,8 +3540,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5486401" y="962025"/>
-          <a:ext cx="3486149" cy="1726536"/>
+          <a:off x="5486402" y="962025"/>
+          <a:ext cx="3865730" cy="1914526"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3281,6 +3767,143 @@
         <a:xfrm>
           <a:off x="6705600" y="962026"/>
           <a:ext cx="2516860" cy="2085974"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>258179</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1356E9D-4B86-4A24-B5E0-AD436C7123D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315201" y="5143500"/>
+          <a:ext cx="4525378" cy="1685925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>198238</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08D54FF1-55E9-43E8-9A5C-7A5F74E38C10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315199" y="8953500"/>
+          <a:ext cx="4465439" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>15666</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{647681F8-CE60-447C-8CFA-C315D4587226}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="11430000"/>
+          <a:ext cx="5886450" cy="968166"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3555,10 +4178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M17"/>
+  <dimension ref="B2:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3571,7 +4194,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -3579,7 +4202,7 @@
         <v>2</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -3633,7 +4256,7 @@
         <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -3655,7 +4278,7 @@
         <v>22</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -3666,7 +4289,7 @@
         <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -3677,7 +4300,7 @@
         <v>24</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
@@ -3688,7 +4311,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
@@ -3707,7 +4330,15 @@
         <v>27</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>404</v>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>502</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -3723,7 +4354,8 @@
     <hyperlink ref="I13" location="S8.Service!A1" display="S8" xr:uid="{E50AE415-15D6-440B-85A4-64AAFBBC8917}"/>
     <hyperlink ref="I15" location="S10.Cloud!A1" display="S10" xr:uid="{0F911F41-8B27-442A-9836-682014819204}"/>
     <hyperlink ref="I14" location="S9.Microservice!A1" display="S9" xr:uid="{7350715F-597E-41F4-85F3-55691363D7BE}"/>
-    <hyperlink ref="I17" location="'S1-3.Overview'!A150" display="'S1-3.Overview'!A150" xr:uid="{1DBD05E7-A39E-4210-A410-C927F7472E59}"/>
+    <hyperlink ref="I17" location="'S1-3.Overview'!A150" display="S1-3!A150" xr:uid="{1DBD05E7-A39E-4210-A410-C927F7472E59}"/>
+    <hyperlink ref="I18" location="Practice!A1" display="Practice" xr:uid="{67406A18-C390-4735-BD17-02A5148A9A0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -3734,8 +4366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB6F0CA-2F5D-4605-8C36-B2178CBE30E9}">
   <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3745,17 +4377,17 @@
         <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4071,22 +4703,22 @@
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E104" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E105" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E106" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E107" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="110" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4117,7 +4749,7 @@
         <v>89</v>
       </c>
       <c r="F115" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
@@ -4125,7 +4757,7 @@
         <v>90</v>
       </c>
       <c r="F116" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
@@ -4135,7 +4767,7 @@
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
@@ -4155,7 +4787,7 @@
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>95</v>
+        <v>500</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
@@ -4165,72 +4797,72 @@
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D136" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D137" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D139" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D140" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D141" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D142" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="146" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4243,52 +4875,52 @@
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C147" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="149" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B149" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C150" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E156" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -4304,10 +4936,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE62828F-30AF-43A0-8C08-890DC7487EDB}">
-  <dimension ref="A1:O190"/>
+  <dimension ref="A1:O191"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4317,17 +4949,17 @@
         <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4340,67 +4972,67 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -4410,42 +5042,42 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="2:15" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4458,637 +5090,637 @@
     </row>
     <row r="46" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C47" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="M47" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="M47" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="N47" s="21"/>
+      <c r="O47" s="16" t="s">
         <v>199</v>
-      </c>
-      <c r="N47" s="19"/>
-      <c r="O47" s="20" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D48" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F48" t="s">
-        <v>194</v>
-      </c>
-      <c r="M48" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="N48" s="17"/>
+        <v>193</v>
+      </c>
+      <c r="M48" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="N48" s="23"/>
       <c r="O48" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F49" t="s">
-        <v>206</v>
-      </c>
-      <c r="M49" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="N49" s="17"/>
+        <v>205</v>
+      </c>
+      <c r="M49" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="N49" s="23"/>
       <c r="O49" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D50" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F50" t="s">
-        <v>195</v>
-      </c>
-      <c r="M50" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="N50" s="17"/>
+        <v>194</v>
+      </c>
+      <c r="M50" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="N50" s="23"/>
       <c r="O50" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="51" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>210</v>
-      </c>
-      <c r="M51" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="N51" s="17"/>
+        <v>209</v>
+      </c>
+      <c r="M51" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="N51" s="23"/>
       <c r="O51" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="56" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D56" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H57" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="62" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
+        <v>237</v>
+      </c>
+      <c r="G73" s="14" t="s">
         <v>238</v>
-      </c>
-      <c r="G73" s="14" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="84" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B84" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
-        <v>242</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>243</v>
+      <c r="C86" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
+      <c r="D88" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C95" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="I95" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C96" s="11" t="s">
+      <c r="C96" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="I96" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C97" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="I97" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D98" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="J98" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D99" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="J99" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D100" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="J100" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>268</v>
+      </c>
+      <c r="J101" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="102" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>210</v>
+      </c>
+      <c r="J102" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="103" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>222</v>
+      </c>
+      <c r="J103" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
         <v>247</v>
       </c>
-      <c r="I96" s="11" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="97" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D97" s="8" t="s">
+      <c r="J104" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="105" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D105" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="J105" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
         <v>274</v>
       </c>
-      <c r="J97" s="8" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="98" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D98" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="J98" s="8" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="99" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D99" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="J99" s="8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="100" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D100" t="s">
-        <v>269</v>
-      </c>
-      <c r="J100" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="101" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D101" t="s">
-        <v>211</v>
-      </c>
-      <c r="J101" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="102" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D102" t="s">
-        <v>223</v>
-      </c>
-      <c r="J102" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="103" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D103" t="s">
-        <v>248</v>
-      </c>
-      <c r="J103" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="104" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D104" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="J104" s="8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="105" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D105" t="s">
-        <v>275</v>
-      </c>
-      <c r="J105" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="106" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D106" t="s">
-        <v>250</v>
-      </c>
       <c r="J106" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="107" spans="4:10" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="107" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J107" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="108" spans="4:10" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="108" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J108" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="109" spans="4:10" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J109" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="110" spans="4:10" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="110" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J110" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="111" spans="4:10" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="111" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J111" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="112" spans="4:10" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="112" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D112" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J112" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="113" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J113" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="J114" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="M114" s="13" t="s">
-        <v>257</v>
+      <c r="D114" t="s">
+        <v>275</v>
+      </c>
+      <c r="J114" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="115" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J115" s="6" t="s">
-        <v>255</v>
+        <v>276</v>
       </c>
       <c r="M115" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="116" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J116" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="118" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C118" t="s">
-        <v>249</v>
-      </c>
-      <c r="J118" t="s">
-        <v>259</v>
+        <v>254</v>
+      </c>
+      <c r="M116" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="117" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J117" s="6" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="119" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J119" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>250</v>
+      </c>
       <c r="J120" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
     </row>
     <row r="121" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J121" t="s">
-        <v>279</v>
-      </c>
-      <c r="O121" s="14" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="122" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J122" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="124" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C124" s="2" t="s">
-        <v>261</v>
+        <v>278</v>
+      </c>
+      <c r="O122" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="123" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J123" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="125" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D125" t="s">
+      <c r="C125" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="126" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="128" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C128" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="127" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C127" s="2" t="s">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="128" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D128" t="s">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E129" t="s">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D130" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E131" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E132" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B135" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C136" t="s">
-        <v>281</v>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B136" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="152" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C152" t="s">
-        <v>285</v>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C140" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="153" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C153" s="11" t="s">
-        <v>287</v>
+      <c r="C153" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="154" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D154" s="8" t="s">
-        <v>273</v>
+      <c r="C154" s="11" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="155" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D155" s="8" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="156" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D156" s="8" t="s">
-        <v>192</v>
+        <v>285</v>
       </c>
     </row>
     <row r="157" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D157" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="159" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C159" t="s">
-        <v>288</v>
+      <c r="D157" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="158" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="160" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="166" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B166" s="5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C168" t="s">
-        <v>293</v>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C164" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B167" s="5" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C169" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C170" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C172" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C171" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="184" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C184" s="8" t="s">
-        <v>302</v>
-      </c>
-    </row>
     <row r="185" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C185" t="s">
-        <v>297</v>
+      <c r="C185" s="8" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="186" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C186" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="187" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C187" t="s">
-        <v>290</v>
-      </c>
-      <c r="I187" s="14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="188" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C188" t="s">
+        <v>289</v>
+      </c>
+      <c r="I188" s="14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="190" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C190" s="8" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="189" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C189" s="8" t="s">
+    <row r="191" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C191" t="s">
         <v>300</v>
-      </c>
-    </row>
-    <row r="190" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C190" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -5115,7 +5747,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5127,10 +5759,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -5143,221 +5775,221 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F14" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D17" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -5374,7 +6006,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5394,47 +6026,47 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="17" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="21" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -5448,9 +6080,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A2D505-2412-4CAE-AA38-79AD3C1C40A3}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5459,7 +6093,7 @@
         <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -5477,338 +6111,396 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>321</v>
+        <v>536</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="11" t="s">
-        <v>334</v>
+        <v>551</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D36" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D37" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D38" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D42" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D43" s="6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D44" s="6" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D45" s="6" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D46" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D47" s="6" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D48" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D49" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" s="6" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>343</v>
+        <v>552</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C59" s="8" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C62" s="13" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C73" s="11" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D74" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D75" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D76" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="11" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="8" t="s">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D78" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D79" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D80" s="6" t="s">
         <v>335</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D76" s="8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="6" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D80" s="6" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D81" s="6" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G81" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D82" s="6" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G82" s="14" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D83" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G83" s="14" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D84" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D85" s="6" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C90" s="12" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>359</v>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C93" s="11" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D96" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -5816,16 +6508,17 @@
     <hyperlink ref="A1" location="Intro!A1" display="Intro!A1" xr:uid="{A4FB059D-59A8-4118-BF6B-FDA60E12987A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1863C95-18D0-4680-8DF0-7B9D3F880515}">
-  <dimension ref="A1:K121"/>
+  <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5835,17 +6528,17 @@
         <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -5858,739 +6551,744 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>401</v>
+      </c>
+      <c r="E7" t="s">
         <v>406</v>
-      </c>
-      <c r="E7" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>402</v>
+      </c>
+      <c r="E8" t="s">
         <v>407</v>
-      </c>
-      <c r="E8" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
+        <v>403</v>
+      </c>
+      <c r="E9" t="s">
         <v>408</v>
-      </c>
-      <c r="E9" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
+        <v>404</v>
+      </c>
+      <c r="E10" t="s">
         <v>409</v>
-      </c>
-      <c r="E10" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
+        <v>405</v>
+      </c>
+      <c r="E11" t="s">
         <v>410</v>
-      </c>
-      <c r="E11" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>417</v>
+      </c>
+      <c r="D25" t="s">
+        <v>418</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="H25" t="s">
         <v>422</v>
-      </c>
-      <c r="D25" t="s">
-        <v>423</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="H25" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="H26" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="I27" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I29" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="11" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="K34" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="K35" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="K36" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="K37" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="K39" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="K40" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="K41" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="K43" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="K44" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="K45" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="K46" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" s="11" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="K49" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="K50" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="K51" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
+        <v>447</v>
+      </c>
+      <c r="K52" t="s">
         <v>452</v>
-      </c>
-      <c r="K52" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="K54" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="55" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="K55" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="56" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="K56" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K57" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="K58" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="K59" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="K60" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="61" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
+        <v>450</v>
+      </c>
+      <c r="K61" t="s">
         <v>455</v>
-      </c>
-      <c r="K61" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="62" spans="4:11" x14ac:dyDescent="0.25">
       <c r="K62" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="63" spans="4:11" x14ac:dyDescent="0.25">
       <c r="K63" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="64" spans="4:11" x14ac:dyDescent="0.25">
       <c r="K64" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="65" spans="3:11" x14ac:dyDescent="0.25">
       <c r="K65" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="66" spans="3:11" x14ac:dyDescent="0.25">
       <c r="K66" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="68" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C68" s="11" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="69" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="70" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="71" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="72" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="73" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="75" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="76" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="77" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="79" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="80" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C80" s="22"/>
+      <c r="C80" s="18"/>
     </row>
     <row r="81" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C81" s="11" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="J81" s="11" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="82" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="K82" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="83" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="K83" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="84" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D84" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="K84" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="85" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
+        <v>466</v>
+      </c>
+      <c r="K85" t="s">
         <v>471</v>
-      </c>
-      <c r="K85" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="86" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="87" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
+        <v>467</v>
+      </c>
+      <c r="K87" t="s">
         <v>472</v>
-      </c>
-      <c r="K87" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="88" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="K88" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="89" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D89" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="K89" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="90" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D90" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="K90" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="91" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D91" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="K91" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="92" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="K92" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="93" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D93" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K93" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="94" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D94" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="K94" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="95" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D95" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="K95" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="97" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C97" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="J97" s="11" t="s">
         <v>480</v>
-      </c>
-      <c r="J97" s="11" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="98" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D98" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="K98" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="99" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="K99" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="100" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D100" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="K100" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="101" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
+        <v>476</v>
+      </c>
+      <c r="K101" t="s">
         <v>481</v>
-      </c>
-      <c r="K101" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="102" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K102" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="103" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
+        <v>477</v>
+      </c>
+      <c r="K103" t="s">
         <v>482</v>
-      </c>
-      <c r="K103" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="104" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="K104" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="105" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D105" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="K105" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="106" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="K106" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="107" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="K107" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="108" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="K108" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="109" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="K109" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="110" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="K110" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="111" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K111" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="112" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D112" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="K112" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="113" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="K113" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="H116" s="14" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="H117" s="14" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="121" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
-        <v>500</v>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="122" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C122" s="1" t="s">
+        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -6599,9 +7297,10 @@
     <hyperlink ref="A1" location="Intro!A1" display="Intro!A1" xr:uid="{93417D2B-5EAE-42A0-BD8E-750385716633}"/>
     <hyperlink ref="D13" r:id="rId1" xr:uid="{21434F2F-F934-4768-9929-6DE191D87F31}"/>
     <hyperlink ref="D14" r:id="rId2" xr:uid="{E8E4B71E-A090-45DB-9971-D3205142C89F}"/>
+    <hyperlink ref="C122" r:id="rId3" xr:uid="{94282B34-1F9B-4804-8247-81798CBBBAA7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -6635,67 +7334,67 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="11" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="H8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="H9" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="H10" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="H11" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -6703,27 +7402,27 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -6734,4 +7433,302 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE519BC-6373-443E-9FD2-49EB5E2AD3C7}">
+  <dimension ref="B2:F66"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="19" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="19" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="19" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="13" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="19" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="19" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="19" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="19" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="19" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="19" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="19" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="19" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="19" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="19" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="19" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="19" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="19"/>
+      <c r="F32" s="13" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="19" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="19" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="19" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="19" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="19" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="19" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="19" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E43" s="19" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="13" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="19" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="13" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="19" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="19" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="19" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="19" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>561</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>